<commit_message>
Update draft tracking tables
</commit_message>
<xml_diff>
--- a/tracking_tables/NMI_structures_tracking_table_template.xlsx
+++ b/tracking_tables/NMI_structures_tracking_table_template.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cwffcf.sharepoint.com/sites/Conservation-General/Shared Documents/Freshwater/Fish Passage/General WCRP/Internal WCRP workshop (2023)/Table and list templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{0D00F7BF-9842-416B-9CF9-E563A1B37C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{136F630A-CD4A-4CE0-BED0-5EEAAFA6FE3F}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{0D00F7BF-9842-416B-9CF9-E563A1B37C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C65CA045-CC39-4DA3-B6D3-6133A76F31AB}"/>
   <bookViews>
-    <workbookView xWindow="-13530" yWindow="15" windowWidth="13530" windowHeight="15570" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
   </bookViews>
   <sheets>
     <sheet name="NMI structures list" sheetId="3" r:id="rId1"/>
     <sheet name="Categories" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NMI structures list'!$H$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NMI structures list'!$I$1:$M$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,53 +39,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={C545E231-C8C5-495F-8764-D237B5782DA9}</author>
-    <author>tc={90A04CE8-0F21-4A37-BF38-4AB0E8015A81}</author>
-  </authors>
-  <commentList>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{C545E231-C8C5-495F-8764-D237B5782DA9}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    this would need to be avg gain for each species </t>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{90A04CE8-0F21-4A37-BF38-4AB0E8015A81}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    this would need to be avg gain for each species </t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={34990351-AABB-47C5-8747-606F813EE6FE}</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{34990351-AABB-47C5-8747-606F813EE6FE}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    As I mentioned in the Confirmed Barriers List tracking table, there might be value in allowing more than one of these to be selected. What if the assessment included habitat and passability assessment? How does it maintain information over multiple visits that would include more than one? </t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Internal Name</t>
   </si>
@@ -96,85 +51,52 @@
     <t>Watercourse Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Easting </t>
+  </si>
+  <si>
+    <t>Northing</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Assessment Step Completed</t>
+  </si>
+  <si>
+    <t>Structure Owner</t>
+  </si>
+  <si>
+    <t>Structure Type</t>
+  </si>
+  <si>
+    <t>Next Steps</t>
+  </si>
+  <si>
+    <t>Lead for Next Steps</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Informal assessment</t>
+  </si>
+  <si>
+    <t>Barrier assessment</t>
+  </si>
+  <si>
+    <t>Habitat confirmation</t>
+  </si>
+  <si>
+    <t>Detailed habitat investigation</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Passage study</t>
+  </si>
+  <si>
     <t>Road Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easting </t>
-  </si>
-  <si>
-    <t>Northing</t>
-  </si>
-  <si>
-    <t>Zone</t>
-  </si>
-  <si>
-    <t>Assessment Step Completed</t>
-  </si>
-  <si>
-    <t>Passability Status</t>
-  </si>
-  <si>
-    <t>Structure Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Habitat Gain (km) </t>
-  </si>
-  <si>
-    <t>Habitat Gain (km) - spawning</t>
-  </si>
-  <si>
-    <t>Habitat Gain (km) - rearing</t>
-  </si>
-  <si>
-    <t>Structure Type</t>
-  </si>
-  <si>
-    <t>Barrier Set Identifier</t>
-  </si>
-  <si>
-    <t>Number of Downstream Barriers</t>
-  </si>
-  <si>
-    <t>Downstream Barrier IDs</t>
-  </si>
-  <si>
-    <t>Upstream Barrier IDs</t>
-  </si>
-  <si>
-    <t>Next Steps</t>
-  </si>
-  <si>
-    <t>Lead for Next Steps</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Assessment complete</t>
-  </si>
-  <si>
-    <t>Next step</t>
-  </si>
-  <si>
-    <t>Informal assessment</t>
-  </si>
-  <si>
-    <t>Barrier assessment</t>
-  </si>
-  <si>
-    <t>Habitat confirmation</t>
-  </si>
-  <si>
-    <t>Detailed habitat investigation</t>
-  </si>
-  <si>
-    <t>Other (with additional field?)</t>
-  </si>
-  <si>
-    <t>Passage study</t>
   </si>
 </sst>
 </file>
@@ -198,7 +120,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -233,6 +155,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -257,9 +180,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Fielding Montgomery" id="{99A25C25-CB7F-48CA-BD57-6FB272204657}" userId="S::fieldingm@cwf-fcf.org::20ab6a0b-133e-45bc-a4ff-27d36bb47b06" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -557,52 +478,27 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L1" dT="2024-01-25T16:15:44.96" personId="{99A25C25-CB7F-48CA-BD57-6FB272204657}" id="{C545E231-C8C5-495F-8764-D237B5782DA9}">
-    <text xml:space="preserve">this would need to be avg gain for each species </text>
-  </threadedComment>
-  <threadedComment ref="M1" dT="2024-01-25T16:15:44.96" personId="{99A25C25-CB7F-48CA-BD57-6FB272204657}" id="{90A04CE8-0F21-4A37-BF38-4AB0E8015A81}">
-    <text xml:space="preserve">this would need to be avg gain for each species </text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2024-02-15T14:51:53.91" personId="{99A25C25-CB7F-48CA-BD57-6FB272204657}" id="{34990351-AABB-47C5-8747-606F813EE6FE}">
-    <text xml:space="preserve">As I mentioned in the Confirmed Barriers List tracking table, there might be value in allowing more than one of these to be selected. What if the assessment included habitat and passability assessment? How does it maintain information over multiple visits that would include more than one? </text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980DA15A-61B7-499A-9DE6-FC999BE847FD}">
-  <dimension ref="A1:U30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980DA15A-61B7-499A-9DE6-FC999BE847FD}">
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="4" width="16.453125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="1" max="5" width="16.453125" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" customWidth="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="9.26953125" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
     <col min="10" max="10" width="21.54296875" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" hidden="1" customWidth="1"/>
-    <col min="12" max="15" width="14.1796875" hidden="1" customWidth="1"/>
-    <col min="16" max="18" width="18" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="23" customWidth="1"/>
-    <col min="21" max="21" width="40.1796875" customWidth="1"/>
+    <col min="11" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="40.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -613,110 +509,52 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -724,22 +562,14 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="4" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -747,22 +577,14 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -770,22 +592,14 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -793,22 +607,14 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -816,22 +622,14 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -839,22 +637,14 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -862,22 +652,14 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-    </row>
-    <row r="10" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -885,22 +667,14 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="1"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-    </row>
-    <row r="11" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -908,22 +682,14 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -931,22 +697,14 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -954,18 +712,11 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="2"/>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -973,18 +724,11 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="1"/>
+      <c r="I14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -992,18 +736,11 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1011,18 +748,11 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="2"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1030,77 +760,69 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="2"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H18" s="2"/>
-      <c r="S18" s="2"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H19" s="2"/>
-      <c r="S19" s="2"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H20" s="2"/>
-      <c r="S20" s="2"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H30" s="2"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{64B7FA89-F364-4DD5-98A8-480ACEC853C6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1346486A-A24F-40FE-A646-B8DE952B449F}">
           <x14:formula1>
-            <xm:f>Categories!$A$2:$A$7</xm:f>
+            <xm:f>Categories!$B$7:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H30</xm:sqref>
+          <xm:sqref>K2:K50</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{59395327-DE8B-4CD2-9930-1ACA4DDB02C3}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{503D6406-CFFA-479C-8FB4-0735ECE0D8C9}">
           <x14:formula1>
-            <xm:f>Categories!$C$2:$C$8</xm:f>
+            <xm:f>Categories!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>S2:S20</xm:sqref>
+          <xm:sqref>I2:I50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1109,68 +831,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4616AE3-541D-40AD-944B-8EAE851DB144}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4616AE3-541D-40AD-944B-8EAE851DB144}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>